<commit_message>
Add to main: 01. /ast_vrfc.py 수정[24.10.26(T_04)], by tamario]
</commit_message>
<xml_diff>
--- a/01_ast_vrfc/02. 자산 검증(24.10)_RSLT.xlsx
+++ b/01_ast_vrfc/02. 자산 검증(24.10)_RSLT.xlsx
@@ -6644,7 +6644,7 @@
   <dimension ref="A1:N266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
@@ -19788,7 +19788,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>

</xml_diff>

<commit_message>
▶ [24.11.01 08:14] 파일 수정(by tamario)
</commit_message>
<xml_diff>
--- a/01_ast_vrfc/02. 자산 검증(24.10)_RSLT.xlsx
+++ b/01_ast_vrfc/02. 자산 검증(24.10)_RSLT.xlsx
@@ -6698,7 +6698,7 @@
       <c r="D3" s="706" t="n"/>
       <c r="E3" s="707" t="inlineStr">
         <is>
-          <t>2024.10.27</t>
+          <t>2024.11.01</t>
         </is>
       </c>
       <c r="G3" s="708" t="inlineStr">
@@ -11792,7 +11792,7 @@
       <c r="H3" s="709" t="n"/>
       <c r="I3" s="707" t="inlineStr">
         <is>
-          <t>2024.10.27</t>
+          <t>2024.11.01</t>
         </is>
       </c>
     </row>

</xml_diff>